<commit_message>
Comit para poder hacer Pull
</commit_message>
<xml_diff>
--- a/OcupacionesI.xlsx
+++ b/OcupacionesI.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Trabajo\Proyectos\Coincidencias\Culture\Impresionismo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34649\Desktop\Impresionismo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{F80DCAC3-F768-42C2-A276-92F57540FE78}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95023316-5249-4102-86B8-DC1F32710392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ocupaciones" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ocupaciones!$A$1:$B$134</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ocupaciones!$A$1:$B$128</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="136">
   <si>
     <t>pintor</t>
   </si>
@@ -773,9 +773,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98539A89-211E-407B-8C8F-069249BD0B88}">
-  <dimension ref="A1:B134"/>
+  <dimension ref="A1:B128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -873,7 +875,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
         <v>133</v>
@@ -881,23 +883,23 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>21</v>
+      <c r="A14" t="s">
+        <v>101</v>
       </c>
       <c r="B14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>132</v>
@@ -905,7 +907,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="B16" t="s">
         <v>132</v>
@@ -913,7 +915,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="B17" t="s">
         <v>132</v>
@@ -921,7 +923,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="B18" t="s">
         <v>132</v>
@@ -929,7 +931,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
         <v>132</v>
@@ -937,7 +939,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B20" t="s">
         <v>132</v>
@@ -945,7 +947,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="B21" t="s">
         <v>132</v>
@@ -953,7 +955,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>107</v>
       </c>
       <c r="B22" t="s">
         <v>132</v>
@@ -961,7 +963,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B23" t="s">
         <v>132</v>
@@ -969,7 +971,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="B24" t="s">
         <v>132</v>
@@ -977,7 +979,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>86</v>
+        <v>9</v>
       </c>
       <c r="B25" t="s">
         <v>132</v>
@@ -985,7 +987,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
       <c r="B26" t="s">
         <v>132</v>
@@ -993,31 +995,31 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="B27" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>69</v>
+      <c r="A28" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>80</v>
+      <c r="A29" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="B30" t="s">
         <v>130</v>
@@ -1025,7 +1027,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>35</v>
+        <v>126</v>
       </c>
       <c r="B31" t="s">
         <v>130</v>
@@ -1033,7 +1035,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>70</v>
+        <v>19</v>
       </c>
       <c r="B32" t="s">
         <v>130</v>
@@ -1041,7 +1043,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>126</v>
+        <v>7</v>
       </c>
       <c r="B33" t="s">
         <v>130</v>
@@ -1049,7 +1051,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B34" t="s">
         <v>130</v>
@@ -1057,7 +1059,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B35" t="s">
         <v>130</v>
@@ -1065,7 +1067,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="B36" t="s">
         <v>130</v>
@@ -1073,7 +1075,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B37" t="s">
         <v>130</v>
@@ -1081,7 +1083,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="B38" t="s">
         <v>130</v>
@@ -1089,7 +1091,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>26</v>
+        <v>118</v>
       </c>
       <c r="B39" t="s">
         <v>130</v>
@@ -1097,7 +1099,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B40" t="s">
         <v>130</v>
@@ -1105,7 +1107,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>118</v>
+        <v>0</v>
       </c>
       <c r="B41" t="s">
         <v>130</v>
@@ -1113,7 +1115,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>62</v>
+        <v>111</v>
       </c>
       <c r="B42" t="s">
         <v>130</v>
@@ -1121,7 +1123,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="B43" t="s">
         <v>130</v>
@@ -1129,7 +1131,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>111</v>
+        <v>57</v>
       </c>
       <c r="B44" t="s">
         <v>130</v>
@@ -1137,7 +1139,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>110</v>
+        <v>36</v>
       </c>
       <c r="B45" t="s">
         <v>130</v>
@@ -1145,7 +1147,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>57</v>
+        <v>116</v>
       </c>
       <c r="B46" t="s">
         <v>130</v>
@@ -1153,7 +1155,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>36</v>
+        <v>103</v>
       </c>
       <c r="B47" t="s">
         <v>130</v>
@@ -1161,23 +1163,23 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>116</v>
+        <v>15</v>
       </c>
       <c r="B48" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>103</v>
+        <v>16</v>
       </c>
       <c r="B49" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>15</v>
+        <v>66</v>
       </c>
       <c r="B50" t="s">
         <v>131</v>
@@ -1185,7 +1187,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="B51" t="s">
         <v>131</v>
@@ -1193,7 +1195,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>66</v>
+        <v>114</v>
       </c>
       <c r="B52" t="s">
         <v>131</v>
@@ -1201,7 +1203,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="B53" t="s">
         <v>131</v>
@@ -1209,7 +1211,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>114</v>
+        <v>72</v>
       </c>
       <c r="B54" t="s">
         <v>131</v>
@@ -1217,7 +1219,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="B55" t="s">
         <v>131</v>
@@ -1225,7 +1227,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>72</v>
+        <v>115</v>
       </c>
       <c r="B56" t="s">
         <v>131</v>
@@ -1233,7 +1235,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B57" t="s">
         <v>131</v>
@@ -1241,7 +1243,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>115</v>
+        <v>87</v>
       </c>
       <c r="B58" t="s">
         <v>131</v>
@@ -1249,7 +1251,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="B59" t="s">
         <v>131</v>
@@ -1257,7 +1259,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="B60" t="s">
         <v>131</v>
@@ -1265,7 +1267,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="B61" t="s">
         <v>131</v>
@@ -1273,7 +1275,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>109</v>
+        <v>27</v>
       </c>
       <c r="B62" t="s">
         <v>131</v>
@@ -1281,7 +1283,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>102</v>
+        <v>34</v>
       </c>
       <c r="B63" t="s">
         <v>131</v>
@@ -1289,7 +1291,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="B64" t="s">
         <v>131</v>
@@ -1297,7 +1299,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="B65" t="s">
         <v>131</v>
@@ -1305,7 +1307,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="B66" t="s">
         <v>131</v>
@@ -1313,31 +1315,31 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>14</v>
+        <v>104</v>
       </c>
       <c r="B67" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B68" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B69" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B70" t="s">
         <v>129</v>
@@ -1345,7 +1347,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="B71" t="s">
         <v>129</v>
@@ -1353,7 +1355,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="B72" t="s">
         <v>129</v>
@@ -1361,39 +1363,39 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>99</v>
+        <v>54</v>
       </c>
       <c r="B73" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
-        <v>25</v>
+      <c r="A74" t="s">
+        <v>81</v>
       </c>
       <c r="B74" t="s">
-        <v>129</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
-        <v>71</v>
+      <c r="A75" t="s">
+        <v>125</v>
       </c>
       <c r="B75" t="s">
-        <v>129</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
-        <v>54</v>
+      <c r="A76" t="s">
+        <v>23</v>
       </c>
       <c r="B76" t="s">
-        <v>129</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>81</v>
+        <v>122</v>
       </c>
       <c r="B77" t="s">
         <v>5</v>
@@ -1401,7 +1403,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>65</v>
+        <v>124</v>
       </c>
       <c r="B78" t="s">
         <v>5</v>
@@ -1409,7 +1411,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>125</v>
+        <v>22</v>
       </c>
       <c r="B79" t="s">
         <v>5</v>
@@ -1417,7 +1419,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="B80" t="s">
         <v>5</v>
@@ -1425,7 +1427,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>122</v>
+        <v>4</v>
       </c>
       <c r="B81" t="s">
         <v>5</v>
@@ -1433,7 +1435,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>124</v>
+        <v>31</v>
       </c>
       <c r="B82" t="s">
         <v>5</v>
@@ -1441,7 +1443,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B83" t="s">
         <v>5</v>
@@ -1449,7 +1451,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
       <c r="B84" t="s">
         <v>5</v>
@@ -1457,7 +1459,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>4</v>
+        <v>92</v>
       </c>
       <c r="B85" t="s">
         <v>5</v>
@@ -1465,7 +1467,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="B86" t="s">
         <v>5</v>
@@ -1473,7 +1475,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="B87" t="s">
         <v>5</v>
@@ -1481,7 +1483,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B88" t="s">
         <v>5</v>
@@ -1489,7 +1491,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>92</v>
+        <v>1</v>
       </c>
       <c r="B89" t="s">
         <v>5</v>
@@ -1497,7 +1499,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>56</v>
+        <v>117</v>
       </c>
       <c r="B90" t="s">
         <v>5</v>
@@ -1505,7 +1507,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>73</v>
+        <v>2</v>
       </c>
       <c r="B91" t="s">
         <v>5</v>
@@ -1513,47 +1515,47 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="B92" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>1</v>
+      <c r="A93" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="B93" t="s">
-        <v>5</v>
+        <v>135</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>117</v>
+      <c r="A94" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="B94" t="s">
-        <v>5</v>
+        <v>135</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>2</v>
+      <c r="A95" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="B95" t="s">
-        <v>5</v>
+        <v>135</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>97</v>
+      <c r="A96" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="B96" t="s">
-        <v>5</v>
+        <v>135</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>50</v>
+        <v>123</v>
       </c>
       <c r="B97" t="s">
         <v>135</v>
@@ -1561,7 +1563,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="B98" t="s">
         <v>135</v>
@@ -1569,7 +1571,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="B99" t="s">
         <v>135</v>
@@ -1577,7 +1579,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>96</v>
+        <v>65</v>
       </c>
       <c r="B100" t="s">
         <v>135</v>
@@ -1585,7 +1587,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="B101" t="s">
         <v>135</v>
@@ -1593,7 +1595,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B102" t="s">
         <v>135</v>
@@ -1601,7 +1603,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="B103" t="s">
         <v>135</v>
@@ -1609,7 +1611,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="B104" t="s">
         <v>135</v>
@@ -1617,7 +1619,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B105" t="s">
         <v>135</v>
@@ -1625,7 +1627,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>59</v>
+        <v>121</v>
       </c>
       <c r="B106" t="s">
         <v>135</v>
@@ -1633,7 +1635,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>38</v>
+        <v>93</v>
       </c>
       <c r="B107" t="s">
         <v>135</v>
@@ -1641,7 +1643,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="B108" t="s">
         <v>135</v>
@@ -1649,7 +1651,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>44</v>
+        <v>84</v>
       </c>
       <c r="B109" t="s">
         <v>135</v>
@@ -1657,7 +1659,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="B110" t="s">
         <v>135</v>
@@ -1665,7 +1667,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>121</v>
+        <v>32</v>
       </c>
       <c r="B111" t="s">
         <v>135</v>
@@ -1673,7 +1675,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>93</v>
+        <v>29</v>
       </c>
       <c r="B112" t="s">
         <v>135</v>
@@ -1681,7 +1683,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>95</v>
+        <v>49</v>
       </c>
       <c r="B113" t="s">
         <v>135</v>
@@ -1689,7 +1691,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>84</v>
+        <v>8</v>
       </c>
       <c r="B114" t="s">
         <v>135</v>
@@ -1697,7 +1699,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
       <c r="B115" t="s">
         <v>135</v>
@@ -1705,7 +1707,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="B116" t="s">
         <v>135</v>
@@ -1713,55 +1715,55 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B117" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="B118" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>8</v>
+        <v>113</v>
       </c>
       <c r="B119" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>78</v>
+        <v>112</v>
       </c>
       <c r="B120" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="B121" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="B122" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>24</v>
+        <v>106</v>
       </c>
       <c r="B123" t="s">
         <v>134</v>
@@ -1769,7 +1771,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="B124" t="s">
         <v>134</v>
@@ -1777,7 +1779,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>113</v>
+        <v>30</v>
       </c>
       <c r="B125" t="s">
         <v>134</v>
@@ -1785,7 +1787,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>112</v>
+        <v>46</v>
       </c>
       <c r="B126" t="s">
         <v>134</v>
@@ -1793,72 +1795,24 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B127" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="2" t="s">
-        <v>53</v>
+      <c r="A128" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="B128" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B129" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B130" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B131" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B132" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B133" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B134" t="s">
-        <v>134</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:B134" xr:uid="{4FECEA65-4659-409A-AC8A-ED27DC500F6F}">
-    <sortState ref="A2:B134">
-      <sortCondition ref="B1:B134"/>
+  <autoFilter ref="A1:B128" xr:uid="{4FECEA65-4659-409A-AC8A-ED27DC500F6F}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B128">
+      <sortCondition ref="B1:B128"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>